<commit_message>
Updated Student term table
</commit_message>
<xml_diff>
--- a/FinalProject.xlsx
+++ b/FinalProject.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533491\Documents\2nd Semester\44663\New folder (2)\Assignment2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533622\Documents\44663\DotnetProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11730" windowHeight="4395" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11730" windowHeight="4395" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="115">
   <si>
     <t>ACS +2</t>
   </si>
@@ -356,6 +356,21 @@
   <si>
     <t>StudentID (varchar(10))(FK)</t>
   </si>
+  <si>
+    <t>FALL2018</t>
+  </si>
+  <si>
+    <t>Sum19</t>
+  </si>
+  <si>
+    <t>Spring2020</t>
+  </si>
+  <si>
+    <t>Sum20</t>
+  </si>
+  <si>
+    <t>Summer2020</t>
+  </si>
 </sst>
 </file>
 
@@ -364,7 +379,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -387,22 +402,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF9CB9C"/>
-        <bgColor rgb="FFF9CB9C"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -440,11 +455,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -456,7 +484,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -473,6 +500,19 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -769,16 +809,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1844,22 +1884,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3126,13 +3166,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4625,7 +4665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -4640,19 +4680,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>104</v>
       </c>
     </row>
@@ -5692,16 +5732,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>90</v>
       </c>
     </row>
@@ -8782,19 +8822,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>95</v>
       </c>
     </row>
@@ -9975,8 +10015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -9990,344 +10030,498 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>3</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>4</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>1</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>1</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>2</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>3</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>4</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>1</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>2</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>3</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>4</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>1</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>2</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>3</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A18" s="6">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>4</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A19" s="6">
+      <c r="A19" s="14">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="15">
         <v>5</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="15" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1"/>
+      <c r="A20" s="16">
+        <v>19</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="18">
+        <v>1</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A21" s="16">
+        <v>20</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="18">
+        <v>2</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A22" s="16">
+        <v>21</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="18">
+        <v>3</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A23" s="16">
+        <v>22</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="18">
+        <v>4</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A24" s="16">
+        <v>23</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="18">
+        <v>5</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A25" s="16">
+        <v>24</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="18">
+        <v>1</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A26" s="16">
+        <v>25</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="18">
+        <v>2</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A27" s="16">
+        <v>26</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="18">
+        <v>3</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A28" s="16">
+        <v>27</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="18">
+        <v>4</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A29" s="16">
+        <v>28</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="18">
+        <v>5</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="31" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="32" spans="1:5" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Created model Updated data
</commit_message>
<xml_diff>
--- a/FinalProject.xlsx
+++ b/FinalProject.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11730" windowHeight="4395" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11730" windowHeight="4395" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="118">
   <si>
     <t>ACS +2</t>
   </si>
@@ -377,6 +377,9 @@
   <si>
     <t>slow And Easy</t>
   </si>
+  <si>
+    <t>string</t>
+  </si>
 </sst>
 </file>
 
@@ -423,7 +426,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -474,11 +477,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -495,7 +511,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -526,6 +541,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -822,16 +844,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>112</v>
       </c>
     </row>
@@ -892,10 +914,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -1903,22 +1925,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3185,13 +3207,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>90</v>
       </c>
     </row>
@@ -4684,7 +4706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -4699,22 +4721,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="15"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="4">
@@ -4732,7 +4754,7 @@
       <c r="E2" s="4">
         <v>4</v>
       </c>
-      <c r="F2" s="15"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="4">
@@ -4750,187 +4772,187 @@
       <c r="E3" s="4">
         <v>4</v>
       </c>
-      <c r="F3" s="15"/>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1">
-      <c r="A4" s="10">
+      <c r="A4" s="9">
         <v>7253</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>533705</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="16">
         <v>3</v>
       </c>
-      <c r="F4" s="15"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1">
-      <c r="A5" s="10">
+      <c r="A5" s="9">
         <v>7254</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>533705</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="16">
         <v>3</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1">
-      <c r="A6" s="10">
+      <c r="A6" s="9">
         <v>7255</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>533491</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <v>3</v>
       </c>
-      <c r="F6" s="15"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <v>7256</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>533491</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="16">
         <v>3</v>
       </c>
-      <c r="F7" s="15"/>
+      <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1">
-      <c r="A8" s="10">
+      <c r="A8" s="9">
         <v>7257</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <v>533727</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="16">
         <v>3</v>
       </c>
-      <c r="F8" s="15"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
-      <c r="A9" s="10">
+      <c r="A9" s="9">
         <v>7258</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>533727</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="16">
         <v>3</v>
       </c>
-      <c r="F9" s="15"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
-      <c r="A10" s="10">
+      <c r="A10" s="9">
         <v>7259</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <v>533622</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="16">
         <v>3</v>
       </c>
-      <c r="F10" s="15"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1">
-      <c r="A11" s="10">
+      <c r="A11" s="9">
         <v>7260</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>533622</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="16">
         <v>3</v>
       </c>
-      <c r="F11" s="15"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1">
-      <c r="A12" s="10">
+      <c r="A12" s="9">
         <v>7261</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <v>533988</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="16">
         <v>3</v>
       </c>
-      <c r="F12" s="15"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1">
-      <c r="A13" s="10">
+      <c r="A13" s="9">
         <v>7262</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <v>533988</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="16">
         <v>3</v>
       </c>
-      <c r="F13" s="15"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -5936,16 +5958,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="8">
+      <c r="D1" s="7">
         <v>919</v>
       </c>
     </row>
@@ -9009,10 +9031,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -9022,27 +9044,31 @@
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="26" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="86.42578125" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="17" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -9055,11 +9081,15 @@
       <c r="D2" s="1">
         <v>542</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="14" t="str">
+        <f>"new Slot{"&amp;$A$1&amp;"="&amp;A2&amp;$B$1&amp;"="&amp;B2&amp;$C$1&amp;"="&amp;C2&amp;$D$1&amp;"="&amp;D2&amp;$E$1&amp;"="&amp;E2</f>
+        <v>new Slot{SlotID(PK)=1DegreePlan(FK)=7251Term=1CreditID(FK)=542Status char(1)=C</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -9072,11 +9102,15 @@
       <c r="D3" s="1">
         <v>563</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="14" t="str">
+        <f t="shared" ref="F3:F12" si="0">"new Slot{"&amp;$A$1&amp;"="&amp;A3&amp;$B$1&amp;"="&amp;B3&amp;$C$1&amp;"="&amp;C3&amp;$D$1&amp;"="&amp;D3&amp;$E$1&amp;"="&amp;E3</f>
+        <v>new Slot{SlotID(PK)=2DegreePlan(FK)=7251Term=1CreditID(FK)=563Status char(1)=C</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -9089,11 +9123,15 @@
       <c r="D4" s="1">
         <v>560</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot{SlotID(PK)=3DegreePlan(FK)=7251Term=1CreditID(FK)=560Status char(1)=C</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -9106,11 +9144,15 @@
       <c r="D5" s="1">
         <v>664</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot{SlotID(PK)=4DegreePlan(FK)=7251Term=2CreditID(FK)=664Status char(1)=A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -9123,11 +9165,15 @@
       <c r="D6" s="1">
         <v>6</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot{SlotID(PK)=5DegreePlan(FK)=7251Term=2CreditID(FK)=6Status char(1)=A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -9140,11 +9186,15 @@
       <c r="D7" s="1">
         <v>10</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot{SlotID(PK)=6DegreePlan(FK)=7251Term=2CreditID(FK)=10Status char(1)=A</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -9157,11 +9207,15 @@
       <c r="D8" s="1">
         <v>618</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="18" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot{SlotID(PK)=7DegreePlan(FK)=7251Term=3CreditID(FK)=618Status char(1)=P</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -9174,11 +9228,15 @@
       <c r="D9" s="1">
         <v>691</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="18" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot{SlotID(PK)=8DegreePlan(FK)=7251Term=3CreditID(FK)=691Status char(1)=P</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -9191,11 +9249,15 @@
       <c r="D10" s="1">
         <v>692</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="18" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot{SlotID(PK)=9DegreePlan(FK)=7251Term=4CreditID(FK)=692Status char(1)=P</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -9208,11 +9270,15 @@
       <c r="D11" s="1">
         <v>20</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="18" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot{SlotID(PK)=10DegreePlan(FK)=7251Term=4CreditID(FK)=20Status char(1)=P</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -9225,8 +9291,12 @@
       <c r="D12" s="1">
         <v>555</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="18" t="s">
         <v>39</v>
+      </c>
+      <c r="F12" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot{SlotID(PK)=11DegreePlan(FK)=7251Term=4CreditID(FK)=555Status char(1)=P</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -10219,7 +10289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E995"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
@@ -10243,7 +10313,7 @@
       <c r="C1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>86</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -10339,7 +10409,7 @@
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="4">
@@ -10356,7 +10426,7 @@
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="4">
@@ -10373,7 +10443,7 @@
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C9" s="4">
@@ -10390,7 +10460,7 @@
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="4">
@@ -10540,351 +10610,351 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A19" s="9">
+      <c r="A19" s="8">
         <v>18</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <v>5</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A20" s="10">
+      <c r="A20" s="9">
         <v>19</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <v>1</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A21" s="10">
+      <c r="A21" s="9">
         <v>20</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="9">
         <v>2</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A22" s="10">
+      <c r="A22" s="9">
         <v>21</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="9">
         <v>3</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A23" s="10">
+      <c r="A23" s="9">
         <v>22</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="9">
         <v>4</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A24" s="10">
+      <c r="A24" s="9">
         <v>23</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="9">
         <v>5</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A25" s="10">
+      <c r="A25" s="9">
         <v>24</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="9">
         <v>1</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="9" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A26" s="10">
+      <c r="A26" s="9">
         <v>25</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="9">
         <v>2</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="9" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A27" s="10">
+      <c r="A27" s="9">
         <v>26</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="9">
         <v>3</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A28" s="10">
+      <c r="A28" s="9">
         <v>27</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="9">
         <v>4</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A29" s="10">
+      <c r="A29" s="9">
         <v>28</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="9">
         <v>5</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A30" s="10">
+      <c r="A30" s="9">
         <v>29</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="9">
         <v>1</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A31" s="10">
+      <c r="A31" s="9">
         <v>30</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="9">
         <v>2</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="9" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A32" s="10">
+      <c r="A32" s="9">
         <v>31</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="9">
         <v>3</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="9" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A33" s="10">
+      <c r="A33" s="9">
         <v>32</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="9">
         <v>4</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A34" s="10">
+      <c r="A34" s="9">
         <v>33</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="9">
         <v>1</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A35" s="10">
+      <c r="A35" s="9">
         <v>34</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="9">
         <v>2</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="9" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A36" s="10">
+      <c r="A36" s="9">
         <v>35</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="9">
         <v>3</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A37" s="10">
+      <c r="A37" s="9">
         <v>36</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="9">
         <v>4</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A38" s="10">
+      <c r="A38" s="9">
         <v>37</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="9">
         <v>5</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="41" spans="1:5" ht="15.75" customHeight="1"/>

</xml_diff>